<commit_message>
Minor updates to documentation
</commit_message>
<xml_diff>
--- a/Support Documentation/Design/Database Details/Data Dictionary.xlsx
+++ b/Support Documentation/Design/Database Details/Data Dictionary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b23540b5940dc24b/Documents/GitHub/pet-adoption-platform/Support Documentation/Design/Database/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b23540b5940dc24b/Documents/GitHub/pet-adoption-platform/Support Documentation/Design/Database Details/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="525" documentId="13_ncr:1_{C1B0FE99-43D3-4C83-9A70-446CD0ACE2CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0609DB5A-48C9-4516-B1FB-EF15151C6D27}"/>
+  <xr:revisionPtr revIDLastSave="527" documentId="13_ncr:1_{C1B0FE99-43D3-4C83-9A70-446CD0ACE2CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3584B5E8-A628-450D-923F-0170481E8601}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{53CEDAC0-C0B7-4620-9FC4-13FBD529EB5A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{53CEDAC0-C0B7-4620-9FC4-13FBD529EB5A}"/>
   </bookViews>
   <sheets>
     <sheet name="Entities" sheetId="1" r:id="rId1"/>
@@ -547,36 +547,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="7">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <b/>
@@ -667,6 +646,27 @@
         <scheme val="minor"/>
       </font>
     </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -735,12 +735,16 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D9C9FD4D-5ECC-4562-84A9-43FF2C96BBC9}" name="Table5" displayName="Table5" ref="A3:D8" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D9C9FD4D-5ECC-4562-84A9-43FF2C96BBC9}" name="Table5" displayName="Table5" ref="A3:D8" totalsRowShown="0" headerRowDxfId="6">
   <autoFilter ref="A3:D8" xr:uid="{D9C9FD4D-5ECC-4562-84A9-43FF2C96BBC9}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{0F0C2776-03D6-4C4B-8FA1-7285B22C7862}" name="Entities"/>
-    <tableColumn id="2" xr3:uid="{5AC8FBF0-0672-40EE-AC9B-9DE0E93138FF}" name="Description" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{5AC8FBF0-0672-40EE-AC9B-9DE0E93138FF}" name="Description" dataDxfId="5"/>
     <tableColumn id="3" xr3:uid="{4C6C88F2-8F3C-4A20-A26B-B30994E91779}" name="DD Complete?"/>
     <tableColumn id="4" xr3:uid="{E6DA9D7F-8C42-4952-ADBC-7F04C41AFA93}" name="ERD Complete?"/>
   </tableColumns>
@@ -749,7 +753,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{2F851650-791A-4B1B-AD76-4200E4AD3FB8}" name="Table134" displayName="Table134" ref="A3:H14" totalsRowShown="0" headerRowDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{2F851650-791A-4B1B-AD76-4200E4AD3FB8}" name="Table134" displayName="Table134" ref="A3:H14" totalsRowShown="0" headerRowDxfId="4">
   <autoFilter ref="A3:H14" xr:uid="{4B623F3C-D3CF-40EF-9EB9-273E09D1438E}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{481A897D-79ED-4701-A306-8AE478D3E8D1}" name="Column Name"/>
@@ -766,7 +770,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4B623F3C-D3CF-40EF-9EB9-273E09D1438E}" name="Table1" displayName="Table1" ref="A3:H13" totalsRowShown="0" headerRowDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4B623F3C-D3CF-40EF-9EB9-273E09D1438E}" name="Table1" displayName="Table1" ref="A3:H13" totalsRowShown="0" headerRowDxfId="3">
   <autoFilter ref="A3:H13" xr:uid="{4B623F3C-D3CF-40EF-9EB9-273E09D1438E}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{1E9FD76C-67CF-4C3A-B2FF-7F27BC227782}" name="Column Name"/>
@@ -783,7 +787,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EC571A79-7597-4ED5-B7C7-7BAE304AE8C8}" name="Table13" displayName="Table13" ref="A3:H8" totalsRowShown="0" headerRowDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EC571A79-7597-4ED5-B7C7-7BAE304AE8C8}" name="Table13" displayName="Table13" ref="A3:H8" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="A3:H8" xr:uid="{4B623F3C-D3CF-40EF-9EB9-273E09D1438E}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{EB709C33-59D5-425D-8377-7248B32C02CE}" name="Column Name"/>
@@ -800,7 +804,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{4607B877-37BB-47F2-8507-417D87380272}" name="Table134567" displayName="Table134567" ref="A3:H8" totalsRowShown="0" headerRowDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{4607B877-37BB-47F2-8507-417D87380272}" name="Table134567" displayName="Table134567" ref="A3:H8" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="A3:H8" xr:uid="{4B623F3C-D3CF-40EF-9EB9-273E09D1438E}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{FBEFA340-7F68-401A-9E6D-41F0196FC817}" name="Column Name"/>
@@ -817,7 +821,7 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{61699D4B-2716-4CCA-90DA-A05266540E53}" name="Table1345675" displayName="Table1345675" ref="A3:H27" totalsRowShown="0" headerRowDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{61699D4B-2716-4CCA-90DA-A05266540E53}" name="Table1345675" displayName="Table1345675" ref="A3:H27" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="A3:H27" xr:uid="{4B623F3C-D3CF-40EF-9EB9-273E09D1438E}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{909BEE94-68FC-428D-B165-D3EFFE5B968F}" name="Column Name"/>
@@ -1152,7 +1156,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1EB38A2-ED52-43FF-841F-8E6F88246B9B}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1163,9 +1169,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="5" t="s">
         <v>146</v>
       </c>
+      <c r="B1" s="5"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1190,7 +1197,7 @@
       <c r="A4" t="s">
         <v>64</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>59</v>
       </c>
       <c r="C4" t="s">
@@ -1204,7 +1211,7 @@
       <c r="A5" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C5" t="s">
@@ -1218,7 +1225,7 @@
       <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>37</v>
       </c>
       <c r="C6" t="s">
@@ -1232,7 +1239,7 @@
       <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C7" t="s">
@@ -1246,13 +1253,13 @@
       <c r="A8" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="4" t="s">
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1267,6 +1274,9 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
   <tableParts count="1">
@@ -2060,7 +2070,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>